<commit_message>
Added union_by option to union, added validations to union
</commit_message>
<xml_diff>
--- a/tests/tables.xlsx
+++ b/tests/tables.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DF0493-953E-482B-B9D3-9EF4E532516C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD112A4-3410-47BB-B32D-405D98A38A49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -155,6 +155,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -439,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +530,7 @@
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -566,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC784604-C8E1-4D45-B8F3-1CCAE139178D}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>